<commit_message>
Update provided fremont-poplar files
</commit_message>
<xml_diff>
--- a/03_test_data/fremont-poplar-data/data/Saturated Water Content_01.xlsx
+++ b/03_test_data/fremont-poplar-data/data/Saturated Water Content_01.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10916"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://desertbotanicalgarden-my.sharepoint.com/personal/dkoepke_dbg_org/Documents/Desktop/Summer 2012 work-related/Macro Study/Macro 2021/Potted cottonwood plant study/Soil/soil, root, leaf model/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/colinpannikkat/Documents/schoolwork/FEL/garisom/03_test_data/fremont-poplar-data/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="123" documentId="8_{E157A70C-4979-482E-A2E3-48E618C5FB23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{61CE17F4-EE96-42DE-B35C-EFB23C8C8A0D}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{214A6B2E-AB2C-7644-B9C8-1978C1730D0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38290" yWindow="-110" windowWidth="38620" windowHeight="21100" activeTab="1" xr2:uid="{EFC7ED9C-9CC9-4939-91D4-CCE385A341BA}"/>
+    <workbookView xWindow="41120" yWindow="-18280" windowWidth="33600" windowHeight="37300" activeTab="1" xr2:uid="{EFC7ED9C-9CC9-4939-91D4-CCE385A341BA}"/>
   </bookViews>
   <sheets>
     <sheet name="Two methods" sheetId="1" r:id="rId1"/>
     <sheet name="Tin method" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" iterate="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -73,7 +73,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Dan Koepke:</t>
         </r>
@@ -82,7 +82,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 The height measured in the pot, using a ruler and tapping to the base of the pot. It is the depth of the soil in the pot.
@@ -307,7 +307,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Dan Koepke:</t>
         </r>
@@ -316,7 +316,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 Height of soil in pvc tube, after pounding the pvc into the soil. The soil heoght seemed to change from the h measurement taken in the pot.
@@ -681,7 +681,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Dan Koepke:</t>
         </r>
@@ -690,7 +690,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 Vsolid.cm3 = Volume of the soil 
@@ -955,7 +955,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Dan Koepke:</t>
         </r>
@@ -964,7 +964,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 BD = SoilDryWght.g/Vtotal.cm3
@@ -1261,7 +1261,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Dan Koepke:</t>
         </r>
@@ -1270,7 +1270,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 Vsolid.cm3 = Volume of the soil 
@@ -1861,7 +1861,7 @@
     <numFmt numFmtId="165" formatCode="0.0"/>
     <numFmt numFmtId="166" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="17" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1910,19 +1910,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
     </font>
     <font>
       <b/>
@@ -2035,26 +2022,26 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="166" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="2" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="1" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="1" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="166" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -4367,9 +4354,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -4407,7 +4394,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -4513,7 +4500,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -4655,7 +4642,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -4669,68 +4656,68 @@
       <selection activeCell="B44" sqref="B44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="15.36328125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.54296875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.1796875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.83203125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="10" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="9" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.1796875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.1640625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="10" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.08984375" bestFit="1" customWidth="1"/>
-    <col min="13" max="14" width="13.36328125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12.6328125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="11.36328125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="13.36328125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="12.6328125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="10.90625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="9.90625" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="16.453125" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="14.1796875" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="14.1796875" customWidth="1"/>
-    <col min="25" max="25" width="14.81640625" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="14.6328125" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="13.54296875" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="14.81640625" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="13.6328125" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="16.1796875" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="14.1796875" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="16.6328125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="10.83203125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="9.83203125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="14.1640625" customWidth="1"/>
+    <col min="25" max="25" width="14.83203125" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="14.83203125" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="16.1640625" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="16.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="2" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="3" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="4" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="5" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:31" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="6" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A6" s="8" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="7" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>0</v>
       </c>
@@ -4825,7 +4812,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="8" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>241212</v>
       </c>
@@ -4939,7 +4926,7 @@
         <v>1.0013203157488975</v>
       </c>
     </row>
-    <row r="9" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>241212</v>
       </c>
@@ -5052,7 +5039,7 @@
         <v>0.34983951955351705</v>
       </c>
     </row>
-    <row r="10" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>241212</v>
       </c>
@@ -5165,7 +5152,7 @@
         <v>0.64777759283125746</v>
       </c>
     </row>
-    <row r="11" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>241212</v>
       </c>
@@ -5278,10 +5265,10 @@
         <v>1.005382519613822</v>
       </c>
     </row>
-    <row r="12" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:31" x14ac:dyDescent="0.2">
       <c r="X12" s="5"/>
     </row>
-    <row r="13" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:31" x14ac:dyDescent="0.2">
       <c r="Q13" s="3" t="s">
         <v>49</v>
       </c>
@@ -5302,7 +5289,7 @@
         <v>0.26354329181394426</v>
       </c>
     </row>
-    <row r="14" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>83</v>
       </c>
@@ -5322,22 +5309,22 @@
         <v>7.0320199647896348E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="16" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="18" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A18" s="8" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="19" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>0</v>
       </c>
@@ -5432,7 +5419,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="20" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>241212</v>
       </c>
@@ -5545,7 +5532,7 @@
       <c r="AG20" s="6"/>
       <c r="AH20" s="12"/>
     </row>
-    <row r="21" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>241212</v>
       </c>
@@ -5658,7 +5645,7 @@
       <c r="AG21" s="6"/>
       <c r="AH21" s="12"/>
     </row>
-    <row r="22" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>241212</v>
       </c>
@@ -5771,7 +5758,7 @@
       <c r="AG22" s="6"/>
       <c r="AH22" s="12"/>
     </row>
-    <row r="23" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>241212</v>
       </c>
@@ -5884,7 +5871,7 @@
       <c r="AG23" s="6"/>
       <c r="AH23" s="12"/>
     </row>
-    <row r="24" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>241212</v>
       </c>
@@ -5997,7 +5984,7 @@
       <c r="AG24" s="6"/>
       <c r="AH24" s="12"/>
     </row>
-    <row r="25" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>241212</v>
       </c>
@@ -6110,7 +6097,7 @@
       <c r="AG25" s="6"/>
       <c r="AH25" s="12"/>
     </row>
-    <row r="26" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>241212</v>
       </c>
@@ -6223,7 +6210,7 @@
       <c r="AG26" s="6"/>
       <c r="AH26" s="12"/>
     </row>
-    <row r="27" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>241212</v>
       </c>
@@ -6336,7 +6323,7 @@
       <c r="AG27" s="6"/>
       <c r="AH27" s="12"/>
     </row>
-    <row r="29" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A29" s="3" t="s">
         <v>49</v>
       </c>
@@ -6365,7 +6352,7 @@
         <v>0.88254687473582771</v>
       </c>
     </row>
-    <row r="30" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A30" s="3" t="s">
         <v>50</v>
       </c>
@@ -6394,38 +6381,38 @@
         <v>3.7953578610563296E-2</v>
       </c>
     </row>
-    <row r="31" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:34" x14ac:dyDescent="0.2">
       <c r="V31" s="5"/>
     </row>
-    <row r="32" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:34" x14ac:dyDescent="0.2">
       <c r="V32" s="5"/>
       <c r="AC32" s="12">
         <v>0.30929725986481971</v>
       </c>
     </row>
-    <row r="33" spans="22:29" x14ac:dyDescent="0.35">
+    <row r="33" spans="22:29" x14ac:dyDescent="0.2">
       <c r="V33" s="5"/>
       <c r="AC33" s="12">
         <v>2.8810699944295165E-2</v>
       </c>
     </row>
-    <row r="34" spans="22:29" x14ac:dyDescent="0.35">
+    <row r="34" spans="22:29" x14ac:dyDescent="0.2">
       <c r="V34" s="5"/>
     </row>
-    <row r="35" spans="22:29" x14ac:dyDescent="0.35">
+    <row r="35" spans="22:29" x14ac:dyDescent="0.2">
       <c r="V35" s="5"/>
     </row>
-    <row r="36" spans="22:29" x14ac:dyDescent="0.35">
+    <row r="36" spans="22:29" x14ac:dyDescent="0.2">
       <c r="V36" s="5"/>
     </row>
-    <row r="37" spans="22:29" x14ac:dyDescent="0.35">
+    <row r="37" spans="22:29" x14ac:dyDescent="0.2">
       <c r="V37" s="5"/>
     </row>
-    <row r="38" spans="22:29" x14ac:dyDescent="0.35">
+    <row r="38" spans="22:29" x14ac:dyDescent="0.2">
       <c r="V38" s="5"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="11" type="noConversion"/>
+  <phoneticPr fontId="9" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
@@ -6440,38 +6427,38 @@
       <selection activeCell="C37" sqref="C37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="16.08984375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.26953125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.1796875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.83203125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="10" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="9" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.1796875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.36328125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.6328125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="8.7265625" customWidth="1"/>
-    <col min="14" max="14" width="10.90625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="9.90625" bestFit="1" customWidth="1"/>
-    <col min="16" max="17" width="8.7265625" customWidth="1"/>
-    <col min="18" max="18" width="9.6328125" customWidth="1"/>
-    <col min="19" max="19" width="14.36328125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="13.1796875" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="13.26953125" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="14.36328125" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="16.26953125" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="14.81640625" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="14.6328125" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="13.54296875" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="14.81640625" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="13.6328125" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="16.1796875" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="14.1796875" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="16.6328125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.6640625" customWidth="1"/>
+    <col min="14" max="14" width="10.83203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="9.83203125" bestFit="1" customWidth="1"/>
+    <col min="16" max="17" width="8.6640625" customWidth="1"/>
+    <col min="18" max="18" width="9.6640625" customWidth="1"/>
+    <col min="19" max="19" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="14.83203125" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="14.83203125" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="16.1640625" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="16.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
@@ -6542,7 +6529,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>241212</v>
       </c>
@@ -6622,7 +6609,7 @@
         <v>0.97215412446954197</v>
       </c>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>241212</v>
       </c>
@@ -6702,7 +6689,7 @@
         <v>1.0055455052665394</v>
       </c>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>241212</v>
       </c>
@@ -6782,7 +6769,7 @@
         <v>0.75870289279253389</v>
       </c>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>241212</v>
       </c>
@@ -6862,7 +6849,7 @@
         <v>0.74475459448492731</v>
       </c>
     </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>241212</v>
       </c>
@@ -6942,7 +6929,7 @@
         <v>0.8652171707778924</v>
       </c>
     </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>241212</v>
       </c>
@@ -7022,7 +7009,7 @@
         <v>0.78575413799516458</v>
       </c>
     </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>241212</v>
       </c>
@@ -7102,7 +7089,7 @@
         <v>0.9742675030009974</v>
       </c>
     </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>241212</v>
       </c>
@@ -7182,7 +7169,7 @@
         <v>0.95397906909902441</v>
       </c>
     </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
         <v>49</v>
       </c>
@@ -7211,7 +7198,7 @@
         <v>0.88254687473582771</v>
       </c>
     </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
         <v>50</v>
       </c>
@@ -7240,27 +7227,27 @@
         <v>3.7953578610563296E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A14" s="24" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="16" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
         <v>63</v>
       </c>
@@ -7268,7 +7255,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B19" s="3" t="s">
         <v>84</v>
       </c>
@@ -7276,7 +7263,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B20" s="25" t="s">
         <v>14</v>
       </c>
@@ -7284,17 +7271,17 @@
         <v>65</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="C21" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="C22" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B23" s="25" t="s">
         <v>13</v>
       </c>
@@ -7302,12 +7289,12 @@
         <v>76</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="C24" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B25" s="25" t="s">
         <v>45</v>
       </c>
@@ -7315,27 +7302,27 @@
         <v>70</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="C26" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="C27" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="C28" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="C29" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B30" s="25" t="s">
         <v>41</v>
       </c>
@@ -7343,17 +7330,17 @@
         <v>73</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="C31" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="C32" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B33" s="26" t="s">
         <v>40</v>
       </c>
@@ -7361,22 +7348,22 @@
         <v>77</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="C34" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="C35" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="C36" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>80</v>
       </c>

</xml_diff>